<commit_message>
Updated HTML files, added new images, and modified Flask project files
</commit_message>
<xml_diff>
--- a/project/flask_comment_section/comments.xlsx
+++ b/project/flask_comment_section/comments.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,324 +436,82 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>ID</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
           <t>Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Comment</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Timestamp</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Narane</t>
-        </is>
+      <c r="A2" t="n">
+        <v>6</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>This is very good product</t>
+          <t>Ajmal</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>2025-02-28 17:55:23</t>
+          <t>very good product</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-03-03 19:15:25</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Aruljothi </t>
-        </is>
+      <c r="A3" t="n">
+        <v>4</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>This is not suitable for me.</t>
+          <t>Naren</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>2025-02-28 14:14:32</t>
+          <t>nice product</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-03-03 18:19:00</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>naveen os</t>
-        </is>
+      <c r="A4" t="n">
+        <v>2</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>this is very comfortable</t>
+          <t>Narendran</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>2025-02-28 09:05:16</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>kumaresan</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t xml:space="preserve">this is perfect product
-</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2025-02-28 08:18:17</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>gayathri mam</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> this product is so good</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2025-02-28 08:13:42</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>sudeer</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>kjhfhjghbh</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2025-02-28 08:11:45</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>PARANTHAMAN R</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>hi</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2025-02-28 07:04:34</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>praveen</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t xml:space="preserve">hi </t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2025-02-28 06:30:51</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>narendran</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>good</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2025-02-28 04:49:43</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>pranav</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>hello</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2025-02-28 04:48:37</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>parama</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>this product is so good</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>2025-02-27 11:55:26</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>Ramar</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>hi hellow</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>2025-02-27 11:49:31</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>kethar nath</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>hi bro</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>2025-02-27 11:45:31</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>partha</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>asflflakjd</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>2025-02-27 09:27:56</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
-        <is>
-          <t>PARANTHAMAN R</t>
-        </is>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>ho</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>2025-02-27 09:15:05</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
-        <is>
-          <t>narendran</t>
-        </is>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>hello</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>2025-02-27 09:10:43</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>naveen</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>hello</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>2025-02-27 09:09:22</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
-        <is>
-          <t>PARANTHAMAN R</t>
-        </is>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>hello</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>2025-02-27 09:08:13</t>
+          <t>This is not fit for me it is very tight for me.</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-03-03 18:14:56</t>
         </is>
       </c>
     </row>

</xml_diff>